<commit_message>
[ADD] resource_group (replace resource_category)
</commit_message>
<xml_diff>
--- a/app_creator/fredheim_1 SQL.xlsx
+++ b/app_creator/fredheim_1 SQL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\o16\src\dev\app_creator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4652D1-2F27-40D2-88D8-A9BC5842773E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E542997B-2A2D-4F44-96E0-946A46E856F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="73">
   <si>
     <t>model.dot</t>
   </si>
@@ -284,6 +284,9 @@
   </si>
   <si>
     <t>product.attribute.value</t>
+  </si>
+  <si>
+    <t>resource.booking.type</t>
   </si>
 </sst>
 </file>
@@ -365,11 +368,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -781,7 +783,7 @@
   <dimension ref="A1:O44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -803,46 +805,46 @@
     <col min="15" max="15" width="51.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>47</v>
       </c>
       <c r="E1"/>
       <c r="F1"/>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="7" t="s">
         <v>7</v>
       </c>
     </row>
@@ -856,11 +858,11 @@
         <v>fh_location.id,</v>
       </c>
       <c r="C2" s="1" t="str">
-        <f>IF(H2="",C1,SUBSTITUTE(H2,".","_"))</f>
+        <f t="shared" ref="C2:C19" si="0">IF(H2="",C1,SUBSTITUTE(H2,".","_"))</f>
         <v>fh_location</v>
       </c>
       <c r="D2" s="1" t="str">
-        <f t="shared" ref="D2" si="0">IF(I2="name","id",I2)</f>
+        <f t="shared" ref="D2" si="1">IF(I2="name","id",I2)</f>
         <v>id</v>
       </c>
       <c r="G2" t="s">
@@ -890,11 +892,11 @@
         <v>fh_program.id,</v>
       </c>
       <c r="C3" s="1" t="str">
-        <f>IF(H3="",C2,SUBSTITUTE(H3,".","_"))</f>
+        <f t="shared" si="0"/>
         <v>fh_program</v>
       </c>
       <c r="D3" s="1" t="str">
-        <f t="shared" ref="D3:D10" si="1">IF(I3="name","id",I3)</f>
+        <f t="shared" ref="D3:D10" si="2">IF(I3="name","id",I3)</f>
         <v>id</v>
       </c>
       <c r="F3" t="s">
@@ -911,14 +913,14 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
       <c r="C4" s="1" t="str">
-        <f>IF(H4="",C3,SUBSTITUTE(H4,".","_"))</f>
+        <f t="shared" si="0"/>
         <v>fh_program</v>
       </c>
       <c r="D4" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>price</v>
       </c>
       <c r="I4" t="s">
@@ -932,14 +934,14 @@
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="1" t="str">
-        <f>IF(H5="",C4,SUBSTITUTE(H5,".","_"))</f>
+        <f t="shared" si="0"/>
         <v>fh_program</v>
       </c>
       <c r="D5" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>location_id</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="8" t="s">
         <v>14</v>
       </c>
       <c r="J5" t="s">
@@ -953,11 +955,11 @@
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="1" t="str">
-        <f>IF(H6="",C5,SUBSTITUTE(H6,".","_"))</f>
+        <f t="shared" si="0"/>
         <v>fh_program</v>
       </c>
       <c r="D6" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>session_ids</v>
       </c>
       <c r="I6" t="s">
@@ -983,11 +985,11 @@
         <v>fh_session.date_start,</v>
       </c>
       <c r="C7" s="1" t="str">
-        <f>IF(H7="",C6,SUBSTITUTE(H7,".","_"))</f>
+        <f t="shared" si="0"/>
         <v>fh_session</v>
       </c>
       <c r="D7" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>date_start</v>
       </c>
       <c r="F7" t="s">
@@ -1016,11 +1018,11 @@
         <v>fh_session.date_end,</v>
       </c>
       <c r="C8" s="1" t="str">
-        <f>IF(H8="",C7,SUBSTITUTE(H8,".","_"))</f>
+        <f t="shared" si="0"/>
         <v>fh_session</v>
       </c>
       <c r="D8" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>date_end</v>
       </c>
       <c r="I8" t="s">
@@ -1037,11 +1039,11 @@
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="1" t="str">
-        <f>IF(H9="",C8,SUBSTITUTE(H9,".","_"))</f>
+        <f t="shared" si="0"/>
         <v>fh_session</v>
       </c>
       <c r="D9" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>program_ids</v>
       </c>
       <c r="I9" t="s">
@@ -1067,18 +1069,18 @@
         <v>fh_room_type.id,</v>
       </c>
       <c r="C10" s="1" t="str">
-        <f>IF(H10="",C9,SUBSTITUTE(H10,".","_"))</f>
+        <f t="shared" si="0"/>
         <v>fh_room_type</v>
       </c>
       <c r="D10" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>id</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>70</v>
       </c>
       <c r="F10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H10" t="s">
         <v>26</v>
@@ -1091,14 +1093,14 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
       <c r="C11" s="1" t="str">
-        <f>IF(H11="",C10,SUBSTITUTE(H11,".","_"))</f>
+        <f t="shared" si="0"/>
         <v>fh_room_type</v>
       </c>
       <c r="D11" s="1" t="str">
-        <f t="shared" ref="D11:D31" si="2">IF(I11="name","id",I11)</f>
+        <f t="shared" ref="D11:D31" si="3">IF(I11="name","id",I11)</f>
         <v>price</v>
       </c>
       <c r="I11" t="s">
@@ -1118,11 +1120,11 @@
         <v>fh_room_type.no_of_beds,</v>
       </c>
       <c r="C12" s="1" t="str">
-        <f>IF(H12="",C11,SUBSTITUTE(H12,".","_"))</f>
+        <f t="shared" si="0"/>
         <v>fh_room_type</v>
       </c>
       <c r="D12" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>no_of_beds</v>
       </c>
       <c r="I12" t="s">
@@ -1142,11 +1144,11 @@
         <v>fh_room_type.has_sink,</v>
       </c>
       <c r="C13" s="1" t="str">
-        <f>IF(H13="",C12,SUBSTITUTE(H13,".","_"))</f>
+        <f t="shared" si="0"/>
         <v>fh_room_type</v>
       </c>
       <c r="D13" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>has_sink</v>
       </c>
       <c r="I13" t="s">
@@ -1166,11 +1168,11 @@
         <v>fh_room_type.has_toilet,</v>
       </c>
       <c r="C14" s="1" t="str">
-        <f>IF(H14="",C13,SUBSTITUTE(H14,".","_"))</f>
+        <f t="shared" si="0"/>
         <v>fh_room_type</v>
       </c>
       <c r="D14" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>has_toilet</v>
       </c>
       <c r="I14" t="s">
@@ -1190,11 +1192,11 @@
         <v>fh_room_type.has_shower,</v>
       </c>
       <c r="C15" s="1" t="str">
-        <f>IF(H15="",C14,SUBSTITUTE(H15,".","_"))</f>
+        <f t="shared" si="0"/>
         <v>fh_room_type</v>
       </c>
       <c r="D15" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>has_shower</v>
       </c>
       <c r="I15" t="s">
@@ -1214,11 +1216,11 @@
         <v>fh_room_type.has_bathtub,</v>
       </c>
       <c r="C16" s="1" t="str">
-        <f>IF(H16="",C15,SUBSTITUTE(H16,".","_"))</f>
+        <f t="shared" si="0"/>
         <v>fh_room_type</v>
       </c>
       <c r="D16" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>has_bathtub</v>
       </c>
       <c r="I16" t="s">
@@ -1232,11 +1234,11 @@
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="1" t="str">
-        <f>IF(H17="",C16,SUBSTITUTE(H17,".","_"))</f>
+        <f t="shared" si="0"/>
         <v>fh_room_type</v>
       </c>
       <c r="D17" s="1" t="str">
-        <f t="shared" ref="D17" si="3">IF(I17="name","id",I17)</f>
+        <f t="shared" ref="D17" si="4">IF(I17="name","id",I17)</f>
         <v>option_ids</v>
       </c>
       <c r="I17" t="s">
@@ -1245,14 +1247,14 @@
       <c r="J17" t="s">
         <v>40</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="K17" t="s">
         <v>58</v>
       </c>
-      <c r="M17" s="3" t="s">
+      <c r="M17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <f>C18&amp;"."&amp;D18&amp;" AS x_"&amp;IF(D18="id",C18&amp;"_","")&amp;D18&amp;","</f>
         <v>fh_room_type_option.id AS x_fh_room_type_option_id,</v>
@@ -1262,75 +1264,72 @@
         <v>fh_room_type_option.id,</v>
       </c>
       <c r="C18" s="1" t="str">
-        <f>IF(H18="",C17,SUBSTITUTE(H18,".","_"))</f>
+        <f t="shared" si="0"/>
         <v>fh_room_type_option</v>
       </c>
       <c r="D18" s="1" t="str">
-        <f t="shared" ref="D18" si="4">IF(I18="name","id",I18)</f>
+        <f t="shared" ref="D18" si="5">IF(I18="name","id",I18)</f>
         <v>id</v>
       </c>
-      <c r="E18"/>
       <c r="F18" t="s">
         <v>71</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" t="s">
         <v>58</v>
       </c>
-      <c r="I18" s="3" t="s">
+      <c r="I18" t="s">
         <v>9</v>
       </c>
-      <c r="J18" s="3" t="s">
+      <c r="J18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="1" t="str">
-        <f>IF(H19="",C18,SUBSTITUTE(H19,".","_"))</f>
+        <f t="shared" si="0"/>
         <v>fh_room_type_option</v>
       </c>
       <c r="D19" s="1" t="str">
-        <f t="shared" ref="D19" si="5">IF(I19="name","id",I19)</f>
+        <f t="shared" ref="D19" si="6">IF(I19="name","id",I19)</f>
         <v>room_type_id</v>
       </c>
-      <c r="E19"/>
-      <c r="I19" s="3" t="s">
+      <c r="I19" t="s">
         <v>38</v>
       </c>
-      <c r="J19" s="3" t="s">
+      <c r="J19" t="s">
         <v>15</v>
       </c>
-      <c r="K19" s="3" t="s">
+      <c r="K19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
       <c r="C20" s="1" t="str">
         <f>IF(H20="",C18,SUBSTITUTE(H20,".","_"))</f>
         <v>fh_room_type_option</v>
       </c>
       <c r="D20" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>price</v>
       </c>
-      <c r="E20"/>
-      <c r="I20" s="3" t="s">
+      <c r="I20" t="s">
         <v>12</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="J20" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C21" s="1" t="str">
-        <f>IF(H21="",C20,SUBSTITUTE(H21,".","_"))</f>
+        <f t="shared" ref="C21:C31" si="7">IF(H21="",C20,SUBSTITUTE(H21,".","_"))</f>
         <v>fh_room</v>
       </c>
       <c r="D21" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>code</v>
       </c>
       <c r="E21" t="s">
@@ -1356,11 +1355,11 @@
         <v>fh_room.id,</v>
       </c>
       <c r="C22" s="1" t="str">
-        <f>IF(H22="",C21,SUBSTITUTE(H22,".","_"))</f>
+        <f t="shared" si="7"/>
         <v>fh_room</v>
       </c>
       <c r="D22" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>id</v>
       </c>
       <c r="I22" t="s">
@@ -1380,11 +1379,11 @@
         <v>fh_room.floor,</v>
       </c>
       <c r="C23" s="1" t="str">
-        <f>IF(H23="",C22,SUBSTITUTE(H23,".","_"))</f>
+        <f t="shared" si="7"/>
         <v>fh_room</v>
       </c>
       <c r="D23" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>floor</v>
       </c>
       <c r="I23" t="s">
@@ -1404,11 +1403,11 @@
         <v>fh_room.view,</v>
       </c>
       <c r="C24" s="1" t="str">
-        <f>IF(H24="",C23,SUBSTITUTE(H24,".","_"))</f>
+        <f t="shared" si="7"/>
         <v>fh_room</v>
       </c>
       <c r="D24" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>view</v>
       </c>
       <c r="I24" t="s">
@@ -1420,11 +1419,11 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C25" s="1" t="str">
-        <f>IF(H25="",C24,SUBSTITUTE(H25,".","_"))</f>
+        <f t="shared" si="7"/>
         <v>fh_room</v>
       </c>
       <c r="D25" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>wing</v>
       </c>
       <c r="I25" t="s">
@@ -1438,14 +1437,14 @@
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="1" t="str">
-        <f>IF(H26="",C25,SUBSTITUTE(H26,".","_"))</f>
+        <f t="shared" si="7"/>
         <v>fh_room</v>
       </c>
       <c r="D26" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>location_id</v>
       </c>
-      <c r="I26" s="9" t="s">
+      <c r="I26" s="8" t="s">
         <v>14</v>
       </c>
       <c r="J26" t="s">
@@ -1459,11 +1458,11 @@
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="1" t="str">
-        <f>IF(H27="",C26,SUBSTITUTE(H27,".","_"))</f>
+        <f t="shared" si="7"/>
         <v>fh_room</v>
       </c>
       <c r="D27" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>room_type_id</v>
       </c>
       <c r="I27" t="s">
@@ -1480,11 +1479,11 @@
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="1" t="str">
-        <f>IF(H28="",C27,SUBSTITUTE(H28,".","_"))</f>
+        <f t="shared" si="7"/>
         <v>fh_room</v>
       </c>
       <c r="D28" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>bed_space_ids</v>
       </c>
       <c r="I28" t="s">
@@ -1502,14 +1501,14 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C29" s="1" t="str">
-        <f>IF(H29="",C28,SUBSTITUTE(H29,".","_"))</f>
+        <f t="shared" si="7"/>
         <v>fh_bed_space</v>
       </c>
       <c r="D29" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>id</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E29" s="8" t="s">
         <v>70</v>
       </c>
       <c r="F29" t="s">
@@ -1535,11 +1534,11 @@
         <v>fh_bed_space.type,</v>
       </c>
       <c r="C30" s="1" t="str">
-        <f>IF(H30="",C29,SUBSTITUTE(H30,".","_"))</f>
+        <f t="shared" si="7"/>
         <v>fh_bed_space</v>
       </c>
       <c r="D30" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>type</v>
       </c>
       <c r="I30" t="s">
@@ -1554,14 +1553,14 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C31" s="1" t="str">
-        <f>IF(H31="",C30,SUBSTITUTE(H31,".","_"))</f>
+        <f t="shared" si="7"/>
         <v>fh_bed_space</v>
       </c>
       <c r="D31" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>room_id</v>
       </c>
-      <c r="I31" s="9" t="s">
+      <c r="I31" s="8" t="s">
         <v>42</v>
       </c>
       <c r="J31" t="s">
@@ -1572,7 +1571,7 @@
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="6" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1627,7 +1626,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="6" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>